<commit_message>
GRANDE CURSO DE MACROECONOMETRIA
</commit_message>
<xml_diff>
--- a/data/grid1_upkoqq33.xlsx
+++ b/data/grid1_upkoqq33.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julio\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\_INSPER\Macroeconometria\Macroeconometria_APS1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36627B65-2343-4F01-B4CF-BA7C06A1EFCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232AF1E4-547B-4B46-813F-DE7D748B6B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -943,7 +943,7 @@
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,9 +1074,9 @@
         <f>93.6</f>
         <v>93.6</v>
       </c>
-      <c r="G4" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G4">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H4">
         <f>-3</f>
@@ -1115,9 +1115,9 @@
         <f>93.8</f>
         <v>93.8</v>
       </c>
-      <c r="G5" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G5">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H5">
         <f>-4.4</f>
@@ -1156,9 +1156,9 @@
         <f>94</f>
         <v>94</v>
       </c>
-      <c r="G6" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G6">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H6">
         <f>-5.4</f>
@@ -1197,9 +1197,9 @@
         <f>94.5</f>
         <v>94.5</v>
       </c>
-      <c r="G7" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G7">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H7">
         <f>-4.6</f>
@@ -1238,9 +1238,9 @@
         <f>94.7</f>
         <v>94.7</v>
       </c>
-      <c r="G8" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G8">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H8">
         <f>-3.6</f>
@@ -1279,9 +1279,9 @@
         <f>94.7</f>
         <v>94.7</v>
       </c>
-      <c r="G9" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G9">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H9">
         <f>-2.5</f>
@@ -1320,9 +1320,9 @@
         <f>94.6</f>
         <v>94.6</v>
       </c>
-      <c r="G10" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G10">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H10">
         <f>-1.4</f>
@@ -1361,9 +1361,9 @@
         <f>94.4</f>
         <v>94.4</v>
       </c>
-      <c r="G11" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G11">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H11">
         <f>-0.8</f>
@@ -1402,9 +1402,9 @@
         <f>94.4</f>
         <v>94.4</v>
       </c>
-      <c r="G12" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G12">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H12">
         <f>-0.7</f>
@@ -1443,9 +1443,9 @@
         <f>94.4</f>
         <v>94.4</v>
       </c>
-      <c r="G13" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G13">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H13">
         <f>-1.3</f>
@@ -1484,9 +1484,9 @@
         <f>94.7</f>
         <v>94.7</v>
       </c>
-      <c r="G14" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G14">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H14">
         <f>-1.3</f>
@@ -1525,9 +1525,9 @@
         <f>94.8</f>
         <v>94.8</v>
       </c>
-      <c r="G15" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G15">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H15">
         <f>0.9</f>
@@ -1566,9 +1566,9 @@
         <f>95</f>
         <v>95</v>
       </c>
-      <c r="G16" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G16">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H16">
         <f>2.3</f>
@@ -1607,9 +1607,9 @@
         <f>95.2</f>
         <v>95.2</v>
       </c>
-      <c r="G17" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G17">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H17">
         <f>4.2</f>
@@ -1648,9 +1648,9 @@
         <f>95.4</f>
         <v>95.4</v>
       </c>
-      <c r="G18" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G18">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H18">
         <f>6.1</f>
@@ -1689,9 +1689,9 @@
         <f>95.6</f>
         <v>95.6</v>
       </c>
-      <c r="G19" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G19">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H19">
         <f>6.4</f>
@@ -1730,9 +1730,9 @@
         <f>95.9</f>
         <v>95.9</v>
       </c>
-      <c r="G20" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G20">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H20">
         <f>8</f>
@@ -1771,9 +1771,9 @@
         <f>96.6</f>
         <v>96.6</v>
       </c>
-      <c r="G21" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G21">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H21">
         <f>8.3</f>
@@ -1812,9 +1812,9 @@
         <f>96.9</f>
         <v>96.9</v>
       </c>
-      <c r="G22" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G22">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H22">
         <f>8.8</f>
@@ -1853,9 +1853,9 @@
         <f>96.8</f>
         <v>96.8</v>
       </c>
-      <c r="G23" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="G23">
+        <f>4</f>
+        <v>4</v>
       </c>
       <c r="H23">
         <f>9.1</f>
@@ -4842,9 +4842,9 @@
         <f>59.6</f>
         <v>59.6</v>
       </c>
-      <c r="F96" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F96">
+        <f t="shared" ref="F96:F123" si="0">99.2</f>
+        <v>99.2</v>
       </c>
       <c r="G96">
         <f>4.1</f>
@@ -4883,9 +4883,9 @@
         <f>54</f>
         <v>54</v>
       </c>
-      <c r="F97" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F97">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G97" t="e">
         <f>NA()</f>
@@ -4924,9 +4924,9 @@
         <f>61.3</f>
         <v>61.3</v>
       </c>
-      <c r="F98" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F98">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G98" t="e">
         <f>NA()</f>
@@ -4965,9 +4965,9 @@
         <f>59.6</f>
         <v>59.6</v>
       </c>
-      <c r="F99" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F99">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G99">
         <f>4.1</f>
@@ -5006,9 +5006,9 @@
         <f>59.7</f>
         <v>59.7</v>
       </c>
-      <c r="F100" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F100">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G100" t="e">
         <f>NA()</f>
@@ -5047,9 +5047,9 @@
         <f>41.9</f>
         <v>41.9</v>
       </c>
-      <c r="F101" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F101">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G101" t="e">
         <f>NA()</f>
@@ -5088,9 +5088,9 @@
         <f>45.2</f>
         <v>45.2</v>
       </c>
-      <c r="F102" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F102">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G102">
         <f>4</f>
@@ -5129,9 +5129,9 @@
         <f>57.2</f>
         <v>57.2</v>
       </c>
-      <c r="F103" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F103">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G103" t="e">
         <f>NA()</f>
@@ -5170,9 +5170,9 @@
         <f>33.2</f>
         <v>33.200000000000003</v>
       </c>
-      <c r="F104" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F104">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G104" t="e">
         <f>NA()</f>
@@ -5211,9 +5211,9 @@
         <f>2.5</f>
         <v>2.5</v>
       </c>
-      <c r="F105" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F105">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G105">
         <f>4.1</f>
@@ -5252,9 +5252,9 @@
         <f>60.5</f>
         <v>60.5</v>
       </c>
-      <c r="F106" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F106">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G106" t="e">
         <f>NA()</f>
@@ -5293,9 +5293,9 @@
         <f>59.3</f>
         <v>59.3</v>
       </c>
-      <c r="F107" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F107">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G107" t="e">
         <f>NA()</f>
@@ -5334,9 +5334,9 @@
         <f>49.9</f>
         <v>49.9</v>
       </c>
-      <c r="F108" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F108">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G108">
         <f>4.1</f>
@@ -5375,9 +5375,9 @@
         <f>54.8</f>
         <v>54.8</v>
       </c>
-      <c r="F109" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F109">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G109" t="e">
         <f>NA()</f>
@@ -5416,9 +5416,9 @@
         <f>45.7</f>
         <v>45.7</v>
       </c>
-      <c r="F110" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F110">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G110" t="e">
         <f>NA()</f>
@@ -5457,9 +5457,9 @@
         <f>31.2</f>
         <v>31.2</v>
       </c>
-      <c r="F111" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F111">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G111">
         <f>4.1</f>
@@ -5498,9 +5498,9 @@
         <f>49.9</f>
         <v>49.9</v>
       </c>
-      <c r="F112" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F112">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G112" t="e">
         <f>NA()</f>
@@ -5539,9 +5539,9 @@
         <f>47.4</f>
         <v>47.4</v>
       </c>
-      <c r="F113" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F113">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G113" t="e">
         <f>NA()</f>
@@ -5580,9 +5580,9 @@
         <f>31.9</f>
         <v>31.9</v>
       </c>
-      <c r="F114" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F114">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G114">
         <f>4.1</f>
@@ -5621,9 +5621,9 @@
         <f>36.2</f>
         <v>36.200000000000003</v>
       </c>
-      <c r="F115" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F115">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G115" t="e">
         <f>NA()</f>
@@ -5662,9 +5662,9 @@
         <f>18.7</f>
         <v>18.7</v>
       </c>
-      <c r="F116" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F116">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G116" t="e">
         <f>NA()</f>
@@ -5703,9 +5703,9 @@
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="F117" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F117">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G117">
         <f>4.1</f>
@@ -5744,9 +5744,9 @@
         <f>-22.6</f>
         <v>-22.6</v>
       </c>
-      <c r="F118" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F118">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G118" t="e">
         <f>NA()</f>
@@ -5785,9 +5785,9 @@
         <f>32</f>
         <v>32</v>
       </c>
-      <c r="F119" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F119">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G119" t="e">
         <f>NA()</f>
@@ -5826,9 +5826,9 @@
         <f>25.2</f>
         <v>25.2</v>
       </c>
-      <c r="F120" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F120">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G120">
         <f>4.1</f>
@@ -5867,9 +5867,9 @@
         <f>33.8</f>
         <v>33.799999999999997</v>
       </c>
-      <c r="F121" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F121">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G121" t="e">
         <f>NA()</f>
@@ -5908,9 +5908,9 @@
         <f>31</f>
         <v>31</v>
       </c>
-      <c r="F122" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F122">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G122" t="e">
         <f>NA()</f>
@@ -5949,9 +5949,9 @@
         <f>14.8</f>
         <v>14.8</v>
       </c>
-      <c r="F123" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F123">
+        <f t="shared" si="0"/>
+        <v>99.2</v>
       </c>
       <c r="G123">
         <f>4</f>

</xml_diff>